<commit_message>
add new class for decorete a cell
</commit_message>
<xml_diff>
--- a/Tables/10.2024/Floor_1_Left_wing.xlsx
+++ b/Tables/10.2024/Floor_1_Left_wing.xlsx
@@ -39,7 +39,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -47,13 +47,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,291 +446,488 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="6" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="6" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>102</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>103</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>104</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>105</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>106</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>124</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>125</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>1.10</t>
         </is>
       </c>
-      <c r="D2" s="1" t="n"/>
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>2.10</t>
         </is>
       </c>
-      <c r="E3" s="1" t="n"/>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2" t="n"/>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>3.10</t>
         </is>
       </c>
-      <c r="F4" s="1" t="n"/>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="3" t="n"/>
+      <c r="E4" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
+      <c r="H4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>4.10</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n"/>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>5.10</t>
         </is>
       </c>
-      <c r="H6" s="1" t="n"/>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>6.10</t>
         </is>
       </c>
-      <c r="B7" s="1" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>7.10</t>
         </is>
       </c>
-      <c r="C8" s="1" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="3" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>8.10</t>
         </is>
       </c>
-      <c r="D9" s="1" t="n"/>
+      <c r="B9" s="3" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>9.10</t>
         </is>
       </c>
-      <c r="E10" s="1" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>10.10</t>
         </is>
       </c>
-      <c r="F11" s="1" t="n"/>
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>11.10</t>
         </is>
       </c>
-      <c r="G12" s="1" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="3" t="n"/>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
+      <c r="H12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>12.10</t>
         </is>
       </c>
-      <c r="H13" s="1" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="3" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>13.10</t>
         </is>
       </c>
-      <c r="B14" s="1" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="3" t="n"/>
+      <c r="H14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>14.10</t>
         </is>
       </c>
-      <c r="C15" s="1" t="n"/>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="3" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>15.10</t>
         </is>
       </c>
-      <c r="D16" s="1" t="n"/>
+      <c r="B16" s="3" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>16.10</t>
         </is>
       </c>
-      <c r="E17" s="1" t="n"/>
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>17.10</t>
         </is>
       </c>
-      <c r="F18" s="1" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="3" t="n"/>
+      <c r="E18" s="2" t="n"/>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>18.10</t>
         </is>
       </c>
-      <c r="G19" s="1" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="3" t="n"/>
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="n"/>
+      <c r="H19" s="2" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>19.10</t>
         </is>
       </c>
-      <c r="H20" s="1" t="n"/>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="3" t="n"/>
+      <c r="G20" s="2" t="n"/>
+      <c r="H20" s="2" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>20.10</t>
         </is>
       </c>
-      <c r="B21" s="1" t="n"/>
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="n"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="3" t="n"/>
+      <c r="H21" s="2" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>21.10</t>
         </is>
       </c>
-      <c r="C22" s="1" t="n"/>
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
+      <c r="H22" s="3" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>22.10</t>
         </is>
       </c>
-      <c r="D23" s="1" t="n"/>
+      <c r="B23" s="3" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="n"/>
+      <c r="E23" s="2" t="n"/>
+      <c r="F23" s="2" t="n"/>
+      <c r="G23" s="2" t="n"/>
+      <c r="H23" s="2" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>23.10</t>
         </is>
       </c>
-      <c r="E24" s="1" t="n"/>
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="3" t="n"/>
+      <c r="D24" s="2" t="n"/>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="2" t="n"/>
+      <c r="H24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>24.10</t>
         </is>
       </c>
-      <c r="F25" s="1" t="n"/>
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="3" t="n"/>
+      <c r="E25" s="2" t="n"/>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
+      <c r="H25" s="2" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>25.10</t>
         </is>
       </c>
-      <c r="G26" s="1" t="n"/>
+      <c r="B26" s="2" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="3" t="n"/>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="2" t="n"/>
+      <c r="H26" s="2" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>26.10</t>
         </is>
       </c>
-      <c r="H27" s="1" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
+      <c r="E27" s="2" t="n"/>
+      <c r="F27" s="3" t="n"/>
+      <c r="G27" s="2" t="n"/>
+      <c r="H27" s="2" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>27.10</t>
         </is>
       </c>
-      <c r="B28" s="1" t="n"/>
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n"/>
+      <c r="E28" s="2" t="n"/>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="3" t="n"/>
+      <c r="H28" s="2" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>28.10</t>
         </is>
       </c>
-      <c r="C29" s="1" t="n"/>
+      <c r="B29" s="2" t="n"/>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n"/>
+      <c r="E29" s="2" t="n"/>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="2" t="n"/>
+      <c r="H29" s="3" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>29.10</t>
         </is>
       </c>
-      <c r="D30" s="1" t="n"/>
+      <c r="B30" s="3" t="n"/>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n"/>
+      <c r="E30" s="2" t="n"/>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
+      <c r="H30" s="2" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>30.10</t>
         </is>
       </c>
-      <c r="E31" s="1" t="n"/>
+      <c r="B31" s="2" t="n"/>
+      <c r="C31" s="3" t="n"/>
+      <c r="D31" s="2" t="n"/>
+      <c r="E31" s="2" t="n"/>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="2" t="n"/>
+      <c r="H31" s="2" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>31.10</t>
         </is>
       </c>
-      <c r="F32" s="1" t="n"/>
+      <c r="B32" s="2" t="n"/>
+      <c r="C32" s="2" t="n"/>
+      <c r="D32" s="3" t="n"/>
+      <c r="E32" s="2" t="n"/>
+      <c r="F32" s="2" t="n"/>
+      <c r="G32" s="2" t="n"/>
+      <c r="H32" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>